<commit_message>
Added code to evaluate IS-Sum_1,2,3 and using them as feature vectors. Added analysis (.xlsx file) and updated training dataset
</commit_message>
<xml_diff>
--- a/Scripts/IS-Sum analysis of multiDomains for correct split.xlsx
+++ b/Scripts/IS-Sum analysis of multiDomains for correct split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tiwari/Documents/Lab-Work/Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9105CFE3-33FB-5441-AE87-1751FD360F63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C503FD65-942A-8642-8871-8B6504D36916}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D4308914-71CE-E745-9BD0-4236B8D0E4CF}"/>
   </bookViews>
@@ -10660,7 +10660,7 @@
   <dimension ref="A1:D1499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A2" sqref="A2:A1499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added code to evaluate IS-Sum_2, IS-Sum_3, IS-Sum_4 and updated the algorithm to train and test using 4 feature vectors [L, IS-Sum_2, IS-Sum_3, IS-Sum_4]. Also adding the raw results: AlgorithmResultsOnAllDatasets_Raw_28August2019.txt. Added Analysis of results on  Benchamrk_2, Benchmark_3 and ASTRAL SCOP 30 as well, check corresponding .xlsx files
</commit_message>
<xml_diff>
--- a/Scripts/IS-Sum analysis of multiDomains for correct split.xlsx
+++ b/Scripts/IS-Sum analysis of multiDomains for correct split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tiwari/Documents/Lab-Work/Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C503FD65-942A-8642-8871-8B6504D36916}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0315F3C4-7653-454E-B5D1-121F500C60A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D4308914-71CE-E745-9BD0-4236B8D0E4CF}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="out" localSheetId="0">Sheet1!$A$2:$D$1499</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{10EEDE9B-BAC7-5147-8C88-60738153B367}" name="out" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Tiwari/Documents/Lab-Work/Scripts/out.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/Tiwari/Documents/Lab-Work/Scripts/out.csv" tab="0" comma="1">
       <textFields count="4">
         <textField type="text"/>
         <textField/>
@@ -10659,7 +10659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8FFBA-2222-9240-A40E-6FB2D34180FD}">
   <dimension ref="A1:D1499"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A1499"/>
     </sheetView>
   </sheetViews>

</xml_diff>